<commit_message>
Refactor: Remove old FastAPI application and related files; introduce new client management service with Excel upload functionality
</commit_message>
<xml_diff>
--- a/agenciasdeviajebarranquilla.xlsx
+++ b/agenciasdeviajebarranquilla.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Nombre</t>
   </si>
@@ -144,19 +144,10 @@
     <t>-74.816908</t>
   </si>
   <si>
-    <t>Alejandro silgado</t>
-  </si>
-  <si>
-    <t>pedro jose</t>
-  </si>
-  <si>
-    <t>daniel giraldo</t>
-  </si>
-  <si>
-    <t>ricardo silgado</t>
-  </si>
-  <si>
     <t>edwin camacho</t>
+  </si>
+  <si>
+    <t>300 6120261</t>
   </si>
 </sst>
 </file>
@@ -522,7 +513,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B6" sqref="B4:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,8 +564,8 @@
       <c r="A2" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="2">
-        <v>3104819492</v>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -606,10 +597,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B3" s="2">
-        <v>3104819492</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -641,10 +632,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3104819492</v>
+        <v>38</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -676,10 +667,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="2">
-        <v>3104819492</v>
+        <v>38</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -711,10 +702,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="2">
-        <v>3104819492</v>
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   agenciasdeviajebarranquilla.xlsx 	modified:   main.py
</commit_message>
<xml_diff>
--- a/agenciasdeviajebarranquilla.xlsx
+++ b/agenciasdeviajebarranquilla.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>Nombre</t>
   </si>
@@ -144,10 +144,22 @@
     <t>-74.816908</t>
   </si>
   <si>
-    <t>edwin camacho</t>
-  </si>
-  <si>
     <t>3104819492</t>
+  </si>
+  <si>
+    <t>carlos</t>
+  </si>
+  <si>
+    <t>juan</t>
+  </si>
+  <si>
+    <t>luis</t>
+  </si>
+  <si>
+    <t>marco</t>
+  </si>
+  <si>
+    <t>daniel</t>
   </si>
 </sst>
 </file>
@@ -513,7 +525,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,10 +574,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -597,10 +609,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -632,10 +644,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -667,10 +679,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -702,10 +714,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>